<commit_message>
added gen-excel in make and regerenated more docs
</commit_message>
<xml_diff>
--- a/project/excel/NEAT_schema.xlsx
+++ b/project/excel/NEAT_schema.xlsx
@@ -1371,7 +1371,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1415,34 +1415,11 @@
           <t>classifier__parameters</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>classifier__layers</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>classifier__metrics</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>classifier__optimizer</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>classifier__fit</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
+    </row>
+  </sheetData>
+  <dataValidations count="1">
     <dataValidation sqref="D2:D1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Average,Hadamard,Sum,L1,L2,AbsoluteL1"</formula1>
-    </dataValidation>
-    <dataValidation sqref="J2:J1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>"Adagrad,Adam,Adamax,Nadam,SGD"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1599,7 +1576,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1618,8 +1595,33 @@
           <t>classifierParams__max_iter</t>
         </is>
       </c>
-    </row>
-  </sheetData>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>classifierParams__layers</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>classifierParams__metrics</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>classifierParams__optimizer</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>classifierParams__fit</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="E2:E1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Adagrad,Adam,Adamax,Nadam,SGD"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>